<commit_message>
Organized results.  Removed old files.
</commit_message>
<xml_diff>
--- a/Simple ILA/Results baseline/baseline times.xlsx
+++ b/Simple ILA/Results baseline/baseline times.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12200" yWindow="460" windowWidth="13400" windowHeight="12600"/>
+    <workbookView xWindow="1740" yWindow="460" windowWidth="23860" windowHeight="12600"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,12 +29,54 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Kerk's laptop</t>
   </si>
   <si>
     <t>Kerk's home</t>
+  </si>
+  <si>
+    <t>baseline</t>
+  </si>
+  <si>
+    <t>ILAsolveLIN</t>
+  </si>
+  <si>
+    <t>ILAsolveVFI</t>
+  </si>
+  <si>
+    <t>ILAsolveGSSA</t>
+  </si>
+  <si>
+    <t>ILAsimLIN</t>
+  </si>
+  <si>
+    <t>ILAsimVFI</t>
+  </si>
+  <si>
+    <t>ILAsimGSSA</t>
+  </si>
+  <si>
+    <t>OLGsolveLIN</t>
+  </si>
+  <si>
+    <t>OLGsolveVFI</t>
+  </si>
+  <si>
+    <t>OLGsolveGSSA</t>
+  </si>
+  <si>
+    <t>OLGsimLIN</t>
+  </si>
+  <si>
+    <t>OLGsimVFI</t>
+  </si>
+  <si>
+    <t>OLGsimGSSA</t>
+  </si>
+  <si>
+    <t>Kerk's desktop</t>
   </si>
 </sst>
 </file>
@@ -373,31 +415,106 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="17.6640625" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
         <v>111.436405553016</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
+      <c r="C2">
         <v>101.447907824556</v>
+      </c>
+      <c r="D2">
+        <v>155.007356226095</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>2.54437059920746E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>2163.1343990180098</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on VFI problems
</commit_message>
<xml_diff>
--- a/Simple ILA/Results baseline/baseline times.xlsx
+++ b/Simple ILA/Results baseline/baseline times.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28908"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="29005"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -16,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Kerk's laptop</t>
   </si>
@@ -77,12 +77,22 @@
   </si>
   <si>
     <t>Kerk's desktop</t>
+  </si>
+  <si>
+    <t>Daryl's computer</t>
+  </si>
+  <si>
+    <t>Relative</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0000000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -112,8 +122,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,104 +427,156 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2:XFD2"/>
+      <selection pane="bottomRight" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="12.83203125" style="2"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2">
         <v>111.436405553016</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>101.447907824556</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>155.007356226095</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F2">
+        <v>20.870006689140801</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B3" s="2">
+        <f>C3/C2</f>
+        <v>9.1913275144513942E-5</v>
+      </c>
+      <c r="C3">
+        <v>1.0242485004710001E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B5" s="1">
+        <f>F5/F2</f>
+        <v>2.9930979083545597</v>
+      </c>
+      <c r="F5">
+        <v>62.465973368613</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B6" s="1">
+        <f>C6/C2</f>
+        <v>882.53140594451622</v>
+      </c>
+      <c r="C6">
+        <v>98346.127666106506</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B8" s="1">
+        <f>F8/F2</f>
+        <v>595.22511766399043</v>
+      </c>
+      <c r="F8">
+        <v>12422.3521871921</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B9">
-        <v>2.54437059920746E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B9" s="2">
+        <f>D9/D2</f>
+        <v>1.2889469253580764E-3</v>
+      </c>
+      <c r="D9">
+        <v>0.130760968874471</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
+        <f>D12/D2</f>
+        <v>21.322612219454879</v>
+      </c>
+      <c r="D12">
         <v>2163.1343990180098</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>14</v>
       </c>

</xml_diff>